<commit_message>
forgot to upload my homework after i did it. so here it is
</commit_message>
<xml_diff>
--- a/assn04/Boyko_assn04.xlsx
+++ b/assn04/Boyko_assn04.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewalverson/Google Drive/teaching/programming/2018S/assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesboyko/classes/2020_PracticalProgramming/homework/assn04/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8172AE-2EC6-914B-A2FA-ECA75D463247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57080" yWindow="460" windowWidth="33040" windowHeight="26840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Query</t>
   </si>
@@ -57,16 +58,46 @@
   </si>
   <si>
     <t>Bit score</t>
+  </si>
+  <si>
+    <t>nad4L.fasta</t>
+  </si>
+  <si>
+    <t>Plus/Plus</t>
+  </si>
+  <si>
+    <t>watermelon_nt</t>
+  </si>
+  <si>
+    <t>watermelon.fsa</t>
+  </si>
+  <si>
+    <t>Plus/Minus</t>
+  </si>
+  <si>
+    <t>mt_genomes/*.fasta</t>
+  </si>
+  <si>
+    <t>nr</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>semi-sensitive</t>
+  </si>
+  <si>
+    <t>sensitive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +131,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,7 +230,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,13 +248,32 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -233,6 +289,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -613,11 +670,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,154 +691,262 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="8" t="s">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="9"/>
+      <c r="C5" s="9">
+        <v>303</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9">
+        <v>303</v>
+      </c>
+      <c r="F5" s="10">
+        <v>560</v>
+      </c>
+      <c r="G5" s="10">
+        <v>303</v>
+      </c>
+      <c r="H5" s="11">
+        <v>9.9999999999999996E-165</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="9"/>
+      <c r="C6" s="12">
+        <v>303</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="13">
+        <v>38948</v>
+      </c>
+      <c r="F6" s="12">
+        <v>560</v>
+      </c>
+      <c r="G6" s="12">
+        <v>303</v>
+      </c>
+      <c r="H6" s="14">
+        <v>1.9999999999999999E-162</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="9"/>
+      <c r="C7" s="12">
+        <v>303</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="13">
+        <v>379236</v>
+      </c>
+      <c r="F7" s="12">
+        <v>560</v>
+      </c>
+      <c r="G7" s="12">
+        <v>303</v>
+      </c>
+      <c r="H7" s="14">
+        <v>2.0000000000000001E-161</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="9"/>
+      <c r="C8" s="12">
+        <v>303</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="13">
+        <v>11638289</v>
+      </c>
+      <c r="F8" s="12">
+        <v>560</v>
+      </c>
+      <c r="G8" s="12">
+        <v>303</v>
+      </c>
+      <c r="H8" s="14">
+        <v>5.9999999999999999E-160</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="12">
+        <v>303</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="16">
+        <v>366130</v>
+      </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="9"/>
+      <c r="G9" s="5">
+        <v>547</v>
+      </c>
+      <c r="H9" s="22">
+        <v>9.2699999999999995E-152</v>
+      </c>
+      <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="9"/>
+      <c r="C10" s="12">
+        <v>303</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="16">
+        <v>379236</v>
+      </c>
+      <c r="G10" s="5">
+        <v>634</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.4099999999999999E-180</v>
+      </c>
+      <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" ht="20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="9"/>
+      <c r="C11" s="12">
+        <v>303</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="16">
+        <v>379236</v>
+      </c>
+      <c r="G11" s="5">
+        <v>625</v>
+      </c>
+      <c r="H11" s="6">
+        <v>8.6700000000000005E-178</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12">
+        <v>303</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="16">
+        <v>379236</v>
+      </c>
+      <c r="G12" s="5">
+        <v>387</v>
+      </c>
+      <c r="H12" s="6">
+        <v>3.9899999999999999E-106</v>
+      </c>
+      <c r="I12" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="B5:G8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G8">
     <sortCondition ref="E3:E6"/>
   </sortState>
   <mergeCells count="6">

</xml_diff>